<commit_message>
Push Presentation B$ defense
</commit_message>
<xml_diff>
--- a/presentation/Statistics/Presentation Statistics.xlsx
+++ b/presentation/Statistics/Presentation Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djarvis3\imt_optimization\presentation\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6068E32A-E766-47D2-A290-BA71F9C97251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7914C4-3BB2-4BEB-ADC2-66225030001E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{58F47700-D290-4C19-858C-C1A571C773EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{58F47700-D290-4C19-858C-C1A571C773EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2850,7 +2850,7 @@
   <dimension ref="A1:O1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>